<commit_message>
Add refresh token, final data columns
</commit_message>
<xml_diff>
--- a/empty_table.xlsx
+++ b/empty_table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23229"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50A4E65E-4E12-4FCF-9494-584C8DEB98A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF5052A9-E444-463D-BFB0-4C506DFC917F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Column1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>User Agent</t>
   </si>
 </sst>
 </file>
@@ -83,10 +98,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0A7A11AD-B22C-4C1E-8E50-7E791FFAEA63}" name="History" displayName="History" ref="A1:A2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:A2" xr:uid="{D29D51AA-D1EC-4605-B94E-CCACE0BF9622}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A05BA386-6B10-4A27-939B-12437B1DF4FB}" name="Column1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0A7A11AD-B22C-4C1E-8E50-7E791FFAEA63}" name="History" displayName="History" ref="A1:F2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:F2" xr:uid="{D29D51AA-D1EC-4605-B94E-CCACE0BF9622}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A05BA386-6B10-4A27-939B-12437B1DF4FB}" name="Timestamp"/>
+    <tableColumn id="2" xr3:uid="{B8B249C1-E75C-42FD-B359-6B4F6B57B79A}" name="Context"/>
+    <tableColumn id="3" xr3:uid="{A0E54407-2FF7-4058-BB7E-68896E7134D5}" name="Title"/>
+    <tableColumn id="4" xr3:uid="{1E043B6E-DCCD-4DAA-93EF-8743B8E20F16}" name="Host"/>
+    <tableColumn id="5" xr3:uid="{3DE31327-1507-47AC-ABB5-2E9F9E8280F6}" name="URL"/>
+    <tableColumn id="6" xr3:uid="{0BB7AF88-F66A-48E1-85CC-0AEEAD3BAF29}" name="User Agent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -389,18 +409,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename 'Context' column to 'Tags' and at 4 extra columns for future use
</commit_message>
<xml_diff>
--- a/empty_table.xlsx
+++ b/empty_table.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23308"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF5052A9-E444-463D-BFB0-4C506DFC917F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFEB3961-761E-480E-B316-E452AA4C9418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Timestamp</t>
   </si>
   <si>
-    <t>Context</t>
+    <t>Tags</t>
   </si>
   <si>
     <t>Title</t>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>User Agent</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
   </si>
 </sst>
 </file>
@@ -98,15 +110,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0A7A11AD-B22C-4C1E-8E50-7E791FFAEA63}" name="History" displayName="History" ref="A1:F2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{D29D51AA-D1EC-4605-B94E-CCACE0BF9622}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A05BA386-6B10-4A27-939B-12437B1DF4FB}" name="Timestamp"/>
-    <tableColumn id="2" xr3:uid="{B8B249C1-E75C-42FD-B359-6B4F6B57B79A}" name="Context"/>
-    <tableColumn id="3" xr3:uid="{A0E54407-2FF7-4058-BB7E-68896E7134D5}" name="Title"/>
-    <tableColumn id="4" xr3:uid="{1E043B6E-DCCD-4DAA-93EF-8743B8E20F16}" name="Host"/>
-    <tableColumn id="5" xr3:uid="{3DE31327-1507-47AC-ABB5-2E9F9E8280F6}" name="URL"/>
-    <tableColumn id="6" xr3:uid="{0BB7AF88-F66A-48E1-85CC-0AEEAD3BAF29}" name="User Agent"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7956350F-5DA9-4C9A-9CF1-553F7A3519F5}" name="History" displayName="History" ref="A1:J2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:J2" xr:uid="{94256598-9FFB-4F74-8B09-B7D58E0259B1}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{33A99691-C239-4F63-B475-55D9F099BAC1}" name="Timestamp"/>
+    <tableColumn id="2" xr3:uid="{BE9D2485-0C5E-4312-995E-3186118D6F19}" name="Tags"/>
+    <tableColumn id="3" xr3:uid="{E88D646A-0B0A-44CE-A340-EEAB3FCBA035}" name="Title"/>
+    <tableColumn id="4" xr3:uid="{A05B4203-8230-480A-BA1F-42AE9865FDFE}" name="Host"/>
+    <tableColumn id="5" xr3:uid="{3A77F4CE-8DDE-49EB-8E67-0ED91D2C0401}" name="URL"/>
+    <tableColumn id="6" xr3:uid="{93B6A911-2971-4982-BBA9-E58748DC8774}" name="User Agent"/>
+    <tableColumn id="7" xr3:uid="{01855AD1-EDCF-48EC-9FFB-32F85AD3FE30}" name="E1"/>
+    <tableColumn id="8" xr3:uid="{754DCA2E-E602-474B-A099-8703B743D953}" name="E2"/>
+    <tableColumn id="9" xr3:uid="{2F6F18BF-0C80-4B76-8E30-F35EA5936326}" name="E3"/>
+    <tableColumn id="10" xr3:uid="{499BBC23-5031-4716-A123-CB8715E8A009}" name="E4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -409,23 +425,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,6 +459,18 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>